<commit_message>
+Annotations added + Modified question 2
</commit_message>
<xml_diff>
--- a/Data/Output/Assignment_2.xlsx
+++ b/Data/Output/Assignment_2.xlsx
@@ -6,10 +6,10 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Landing Page" sheetId="2" r:id="rId2"/>
-    <x:sheet name="reading" sheetId="5" r:id="rId5"/>
-    <x:sheet name="inspirational" sheetId="7" r:id="rId7"/>
-    <x:sheet name="friendship" sheetId="8" r:id="rId8"/>
+    <x:sheet name="Quotes" sheetId="2" r:id="rId2"/>
+    <x:sheet name="readingQuotes" sheetId="5" r:id="rId5"/>
+    <x:sheet name="inspirationalQuotes" sheetId="7" r:id="rId7"/>
+    <x:sheet name="friendshipQuotes" sheetId="8" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>

</xml_diff>